<commit_message>
Fixed TC Production Error
</commit_message>
<xml_diff>
--- a/TestWorkbook.xlsx
+++ b/TestWorkbook.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\CHLINUH\Desktop\TestXLTrail\XLTest\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{279C2756-A593-47F8-80DE-9C98C02EC23A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{386966D0-4632-4909-965F-410D46EB079D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Test1" sheetId="1" r:id="rId1"/>
@@ -367,10 +367,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="B4:K13"/>
+  <dimension ref="B4:K26"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="O12" sqref="O12"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="O13" sqref="O13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -557,6 +557,191 @@
     </row>
     <row r="13" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B13">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="17" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B17">
+        <v>1</v>
+      </c>
+      <c r="C17">
+        <v>2</v>
+      </c>
+      <c r="D17">
+        <v>3</v>
+      </c>
+      <c r="E17">
+        <v>4</v>
+      </c>
+      <c r="F17">
+        <v>5</v>
+      </c>
+      <c r="G17">
+        <v>6</v>
+      </c>
+      <c r="H17">
+        <v>7</v>
+      </c>
+      <c r="I17">
+        <v>8</v>
+      </c>
+      <c r="J17">
+        <v>9</v>
+      </c>
+      <c r="K17">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="18" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B18">
+        <v>2</v>
+      </c>
+      <c r="C18">
+        <v>3</v>
+      </c>
+      <c r="D18">
+        <v>4</v>
+      </c>
+      <c r="E18">
+        <v>5</v>
+      </c>
+      <c r="F18">
+        <v>6</v>
+      </c>
+      <c r="G18">
+        <v>7</v>
+      </c>
+      <c r="H18">
+        <v>8</v>
+      </c>
+      <c r="I18">
+        <v>9</v>
+      </c>
+      <c r="J18">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="19" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B19">
+        <v>3</v>
+      </c>
+      <c r="C19">
+        <v>4</v>
+      </c>
+      <c r="D19">
+        <v>5</v>
+      </c>
+      <c r="E19">
+        <v>6</v>
+      </c>
+      <c r="F19">
+        <v>7</v>
+      </c>
+      <c r="G19">
+        <v>8</v>
+      </c>
+      <c r="H19">
+        <v>9</v>
+      </c>
+      <c r="I19">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="20" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B20">
+        <v>4</v>
+      </c>
+      <c r="C20">
+        <v>5</v>
+      </c>
+      <c r="D20">
+        <v>6</v>
+      </c>
+      <c r="E20">
+        <v>7</v>
+      </c>
+      <c r="F20">
+        <v>8</v>
+      </c>
+      <c r="G20">
+        <v>9</v>
+      </c>
+      <c r="H20">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="21" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B21">
+        <v>5</v>
+      </c>
+      <c r="C21">
+        <v>6</v>
+      </c>
+      <c r="D21">
+        <v>7</v>
+      </c>
+      <c r="E21">
+        <v>8</v>
+      </c>
+      <c r="F21">
+        <v>9</v>
+      </c>
+      <c r="G21">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="22" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B22">
+        <v>6</v>
+      </c>
+      <c r="C22">
+        <v>7</v>
+      </c>
+      <c r="D22">
+        <v>8</v>
+      </c>
+      <c r="E22">
+        <v>9</v>
+      </c>
+      <c r="F22">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="23" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B23">
+        <v>7</v>
+      </c>
+      <c r="C23">
+        <v>8</v>
+      </c>
+      <c r="D23">
+        <v>9</v>
+      </c>
+      <c r="E23">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="24" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B24">
+        <v>8</v>
+      </c>
+      <c r="C24">
+        <v>9</v>
+      </c>
+      <c r="D24">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="25" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B25">
+        <v>9</v>
+      </c>
+      <c r="C25">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="26" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B26">
         <v>10</v>
       </c>
     </row>
@@ -570,7 +755,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0A0866D1-E9A6-4AC7-A448-143B0C202EC0}">
   <dimension ref="B4:I21"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="L15" sqref="L15"/>
     </sheetView>
   </sheetViews>

</xml_diff>